<commit_message>
feat: Add UI and integrate with API
</commit_message>
<xml_diff>
--- a/dataset/Job.xlsx
+++ b/dataset/Job.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\IT Career Recommendation\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7FB7B7F-964E-4745-B8FF-F56AF0C26EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC34A217-CE5C-4659-B3F2-D6F99510DD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5C0F0CF8-E217-433B-9DC9-F8BA6C5D06FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{5C0F0CF8-E217-433B-9DC9-F8BA6C5D06FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1341,7 +1341,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1640,20 +1640,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A356" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D377" sqref="D377"/>
+    <sheetView tabSelected="1" topLeftCell="A304" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>44931</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>44967</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>45036</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>45071</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>45112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>45148</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>85</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>45255</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>91</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>96</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>115</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>121</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>126</v>
       </c>
@@ -2293,7 +2294,7 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>131</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>136</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>142</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>146</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>151</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>157</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>167</v>
       </c>
@@ -2549,7 +2550,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>177</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>187</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>191</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>197</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>201</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>207</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>211</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>217</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>221</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>226</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>230</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>234</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>237</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>243</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>246</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>250</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>254</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>263</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>267</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>271</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>275</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>280</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>284</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>288</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>293</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>297</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>301</v>
       </c>
@@ -3509,7 +3510,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>305</v>
       </c>
@@ -3541,7 +3542,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>310</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>45235</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>315</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>319</v>
       </c>
@@ -3637,7 +3638,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>324</v>
       </c>
@@ -3669,7 +3670,7 @@
         <v>44977</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>327</v>
       </c>
@@ -3701,7 +3702,7 @@
         <v>45010</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>331</v>
       </c>
@@ -3733,7 +3734,7 @@
         <v>45046</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>335</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>45051</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>341</v>
       </c>
@@ -3797,7 +3798,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>346</v>
       </c>
@@ -3829,7 +3830,7 @@
         <v>45122</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>348</v>
       </c>
@@ -3861,7 +3862,7 @@
         <v>45158</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>353</v>
       </c>
@@ -3893,7 +3894,7 @@
         <v>45194</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>357</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>45229</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>151</v>
       </c>
@@ -3957,7 +3958,7 @@
         <v>44931</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>364</v>
       </c>
@@ -3989,7 +3990,7 @@
         <v>44967</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>367</v>
       </c>
@@ -4021,7 +4022,7 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>121</v>
       </c>
@@ -4053,7 +4054,7 @@
         <v>45036</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>43</v>
       </c>
@@ -4085,7 +4086,7 @@
         <v>45071</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>50</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>45107</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>57</v>
       </c>
@@ -4149,7 +4150,7 @@
         <v>45112</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>64</v>
       </c>
@@ -4181,7 +4182,7 @@
         <v>45148</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -4213,7 +4214,7 @@
         <v>45184</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -4245,7 +4246,7 @@
         <v>45219</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>45255</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -4309,7 +4310,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -4341,7 +4342,7 @@
         <v>45275</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -4373,7 +4374,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>45285</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>110</v>
       </c>
@@ -4437,7 +4438,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>115</v>
       </c>
@@ -4469,7 +4470,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>121</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>126</v>
       </c>
@@ -4533,7 +4534,7 @@
         <v>45275</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>131</v>
       </c>
@@ -4565,7 +4566,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>136</v>
       </c>
@@ -4597,7 +4598,7 @@
         <v>45285</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>142</v>
       </c>
@@ -4629,7 +4630,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>146</v>
       </c>
@@ -4661,7 +4662,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>151</v>
       </c>
@@ -4693,7 +4694,7 @@
         <v>44566</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>157</v>
       </c>
@@ -4725,7 +4726,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>163</v>
       </c>
@@ -4757,7 +4758,7 @@
         <v>44635</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>167</v>
       </c>
@@ -4789,7 +4790,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>172</v>
       </c>
@@ -4821,7 +4822,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>177</v>
       </c>
@@ -4853,7 +4854,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>182</v>
       </c>
@@ -4885,7 +4886,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>187</v>
       </c>
@@ -4917,7 +4918,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>191</v>
       </c>
@@ -4949,7 +4950,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>197</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>201</v>
       </c>
@@ -5013,7 +5014,7 @@
         <v>44890</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>207</v>
       </c>
@@ -5045,7 +5046,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>211</v>
       </c>
@@ -5077,7 +5078,7 @@
         <v>44910</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>217</v>
       </c>
@@ -5109,7 +5110,7 @@
         <v>44915</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>221</v>
       </c>
@@ -5141,7 +5142,7 @@
         <v>44920</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>226</v>
       </c>
@@ -5173,7 +5174,7 @@
         <v>44925</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>230</v>
       </c>
@@ -5205,7 +5206,7 @@
         <v>44926</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>234</v>
       </c>
@@ -5237,7 +5238,7 @@
         <v>45270</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>237</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>45275</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>243</v>
       </c>
@@ -5301,7 +5302,7 @@
         <v>45280</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>246</v>
       </c>
@@ -5333,7 +5334,7 @@
         <v>45285</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>250</v>
       </c>
@@ -5365,7 +5366,7 @@
         <v>45290</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>254</v>
       </c>
@@ -5397,7 +5398,7 @@
         <v>45291</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>258</v>
       </c>
@@ -5429,7 +5430,7 @@
         <v>44566</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>263</v>
       </c>
@@ -5461,7 +5462,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>267</v>
       </c>
@@ -5493,7 +5494,7 @@
         <v>44635</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>271</v>
       </c>
@@ -5525,7 +5526,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -5557,7 +5558,7 @@
         <v>44566</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>19</v>
       </c>
@@ -5589,7 +5590,7 @@
         <v>44602</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>27</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>44635</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>35</v>
       </c>
@@ -5653,7 +5654,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>43</v>
       </c>
@@ -5685,7 +5686,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>50</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -5749,7 +5750,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>64</v>
       </c>
@@ -5781,7 +5782,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>71</v>
       </c>
@@ -5813,7 +5814,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>78</v>
       </c>
@@ -5845,7 +5846,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>85</v>
       </c>
@@ -5877,7 +5878,7 @@
         <v>44890</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>91</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>96</v>
       </c>
@@ -5941,7 +5942,7 @@
         <v>44910</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>100</v>
       </c>
@@ -5973,7 +5974,7 @@
         <v>44915</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>105</v>
       </c>
@@ -6005,7 +6006,7 @@
         <v>44920</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>110</v>
       </c>
@@ -6037,7 +6038,7 @@
         <v>44925</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>115</v>
       </c>
@@ -6069,7 +6070,7 @@
         <v>44706</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>121</v>
       </c>
@@ -6101,7 +6102,7 @@
         <v>44742</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>126</v>
       </c>
@@ -6133,7 +6134,7 @@
         <v>44747</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>131</v>
       </c>
@@ -6165,7 +6166,7 @@
         <v>44783</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>136</v>
       </c>
@@ -6197,7 +6198,7 @@
         <v>44819</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>142</v>
       </c>
@@ -6229,7 +6230,7 @@
         <v>44854</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>146</v>
       </c>
@@ -6261,7 +6262,7 @@
         <v>44890</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -6293,7 +6294,7 @@
         <v>44905</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>157</v>
       </c>
@@ -6325,7 +6326,7 @@
         <v>44910</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>163</v>
       </c>
@@ -6357,7 +6358,7 @@
         <v>44915</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -6389,7 +6390,7 @@
         <v>44920</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>172</v>
       </c>
@@ -6421,7 +6422,7 @@
         <v>44925</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>177</v>
       </c>
@@ -6453,7 +6454,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>182</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>44928</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>187</v>
       </c>
@@ -6517,7 +6518,7 @@
         <v>44929</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>191</v>
       </c>
@@ -6549,7 +6550,7 @@
         <v>44930</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>197</v>
       </c>
@@ -6581,7 +6582,7 @@
         <v>44931</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>201</v>
       </c>
@@ -6613,7 +6614,7 @@
         <v>44932</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>207</v>
       </c>
@@ -6645,7 +6646,7 @@
         <v>44933</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>211</v>
       </c>
@@ -6677,7 +6678,7 @@
         <v>44934</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>217</v>
       </c>
@@ -6709,7 +6710,7 @@
         <v>44935</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>221</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>44936</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>226</v>
       </c>
@@ -6773,7 +6774,7 @@
         <v>44937</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>230</v>
       </c>
@@ -6805,7 +6806,7 @@
         <v>44938</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>234</v>
       </c>
@@ -6837,7 +6838,7 @@
         <v>44939</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>237</v>
       </c>
@@ -6869,7 +6870,7 @@
         <v>44940</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>243</v>
       </c>
@@ -6901,7 +6902,7 @@
         <v>44941</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>246</v>
       </c>
@@ -6933,7 +6934,7 @@
         <v>44942</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>250</v>
       </c>
@@ -6965,7 +6966,7 @@
         <v>44943</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>254</v>
       </c>
@@ -6997,7 +6998,7 @@
         <v>44944</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>258</v>
       </c>
@@ -7029,7 +7030,7 @@
         <v>44945</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>263</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>267</v>
       </c>
@@ -7093,7 +7094,7 @@
         <v>44947</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>271</v>
       </c>
@@ -7125,7 +7126,7 @@
         <v>44948</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>364</v>
       </c>
@@ -7157,7 +7158,7 @@
         <v>44270</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>19</v>
       </c>
@@ -7189,7 +7190,7 @@
         <v>44306</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>27</v>
       </c>
@@ -7221,7 +7222,7 @@
         <v>44357</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>35</v>
       </c>
@@ -7253,7 +7254,7 @@
         <v>44433</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>43</v>
       </c>
@@ -7285,7 +7286,7 @@
         <v>44474</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>50</v>
       </c>
@@ -7317,7 +7318,7 @@
         <v>44515</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>57</v>
       </c>
@@ -7349,7 +7350,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>243</v>
       </c>
@@ -7381,7 +7382,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>226</v>
       </c>
@@ -7413,7 +7414,7 @@
         <v>44275</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>19</v>
       </c>
@@ -7445,7 +7446,7 @@
         <v>44301</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>27</v>
       </c>
@@ -7477,7 +7478,7 @@
         <v>44328</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>35</v>
       </c>
@@ -7509,7 +7510,7 @@
         <v>44372</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>43</v>
       </c>
@@ -7541,7 +7542,7 @@
         <v>44395</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>50</v>
       </c>
@@ -7573,7 +7574,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>57</v>
       </c>
@@ -7605,7 +7606,7 @@
         <v>44453</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>254</v>
       </c>
@@ -7637,7 +7638,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>258</v>
       </c>
@@ -7669,7 +7670,7 @@
         <v>44509</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>364</v>
       </c>
@@ -7701,7 +7702,7 @@
         <v>44534</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>243</v>
       </c>
@@ -7733,7 +7734,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>226</v>
       </c>
@@ -7765,7 +7766,7 @@
         <v>44275</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>19</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>44301</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>27</v>
       </c>
@@ -7829,7 +7830,7 @@
         <v>44328</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>35</v>
       </c>
@@ -7861,7 +7862,7 @@
         <v>44372</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>43</v>
       </c>
@@ -7893,7 +7894,7 @@
         <v>44395</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>50</v>
       </c>
@@ -7925,7 +7926,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>57</v>
       </c>
@@ -7957,7 +7958,7 @@
         <v>44453</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>254</v>
       </c>
@@ -7989,7 +7990,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>258</v>
       </c>
@@ -8021,7 +8022,7 @@
         <v>44509</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>364</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>44534</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>243</v>
       </c>
@@ -8085,7 +8086,7 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>64</v>
       </c>
@@ -8117,7 +8118,7 @@
         <v>44280</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>409</v>
       </c>
@@ -8149,7 +8150,7 @@
         <v>44305</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>271</v>
       </c>
@@ -8181,7 +8182,7 @@
         <v>44331</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>126</v>
       </c>
@@ -8213,7 +8214,7 @@
         <v>44377</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>115</v>
       </c>
@@ -8245,7 +8246,7 @@
         <v>44399</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>414</v>
       </c>
@@ -8277,7 +8278,7 @@
         <v>44425</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>151</v>
       </c>
@@ -8309,7 +8310,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>131</v>
       </c>
@@ -8341,7 +8342,7 @@
         <v>44471</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>100</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>44527</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>105</v>
       </c>
@@ -8405,7 +8406,7 @@
         <v>44552</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>157</v>
       </c>
@@ -8437,7 +8438,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>163</v>
       </c>
@@ -8469,7 +8470,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>167</v>
       </c>
@@ -8501,7 +8502,7 @@
         <v>44291</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>172</v>
       </c>
@@ -8533,7 +8534,7 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>177</v>
       </c>
@@ -8565,7 +8566,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>182</v>
       </c>
@@ -8597,7 +8598,7 @@
         <v>44391</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>187</v>
       </c>
@@ -8629,7 +8630,7 @@
         <v>44417</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>191</v>
       </c>
@@ -8661,7 +8662,7 @@
         <v>44443</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>197</v>
       </c>
@@ -8693,7 +8694,7 @@
         <v>44499</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>201</v>
       </c>
@@ -8725,7 +8726,7 @@
         <v>44525</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>207</v>
       </c>
@@ -8757,7 +8758,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>211</v>
       </c>
@@ -8789,7 +8790,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>217</v>
       </c>
@@ -8821,7 +8822,7 @@
         <v>44274</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>221</v>
       </c>
@@ -8853,7 +8854,7 @@
         <v>44300</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>226</v>
       </c>
@@ -8885,7 +8886,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>230</v>
       </c>
@@ -8917,7 +8918,7 @@
         <v>44353</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>157</v>
       </c>
@@ -8949,7 +8950,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>237</v>
       </c>
@@ -8981,7 +8982,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>243</v>
       </c>
@@ -9013,7 +9014,7 @@
         <v>44461</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>246</v>
       </c>
@@ -9045,7 +9046,7 @@
         <v>44487</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>250</v>
       </c>
@@ -9077,7 +9078,7 @@
         <v>44513</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>254</v>
       </c>
@@ -9109,7 +9110,7 @@
         <v>44539</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>243</v>
       </c>
@@ -9141,7 +9142,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>226</v>
       </c>
@@ -9173,7 +9174,7 @@
         <v>44275</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>19</v>
       </c>
@@ -9205,7 +9206,7 @@
         <v>44301</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>27</v>
       </c>
@@ -9237,7 +9238,7 @@
         <v>44328</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>35</v>
       </c>
@@ -9269,7 +9270,7 @@
         <v>44372</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>43</v>
       </c>
@@ -9301,7 +9302,7 @@
         <v>44395</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>50</v>
       </c>
@@ -9333,7 +9334,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>57</v>
       </c>
@@ -9365,7 +9366,7 @@
         <v>44453</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>254</v>
       </c>
@@ -9397,7 +9398,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>258</v>
       </c>
@@ -9429,7 +9430,7 @@
         <v>44509</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>364</v>
       </c>
@@ -9461,7 +9462,7 @@
         <v>44534</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>243</v>
       </c>
@@ -9493,7 +9494,7 @@
         <v>44255</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>64</v>
       </c>
@@ -9525,7 +9526,7 @@
         <v>44280</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>409</v>
       </c>
@@ -9557,7 +9558,7 @@
         <v>44305</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>271</v>
       </c>
@@ -9589,7 +9590,7 @@
         <v>44331</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>126</v>
       </c>
@@ -9621,7 +9622,7 @@
         <v>44377</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>115</v>
       </c>
@@ -9653,7 +9654,7 @@
         <v>44399</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>414</v>
       </c>
@@ -9685,7 +9686,7 @@
         <v>44425</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>151</v>
       </c>
@@ -9717,7 +9718,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>131</v>
       </c>
@@ -9749,7 +9750,7 @@
         <v>44471</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>100</v>
       </c>
@@ -9781,7 +9782,7 @@
         <v>44527</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>105</v>
       </c>
@@ -9813,7 +9814,7 @@
         <v>44552</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>157</v>
       </c>
@@ -9845,7 +9846,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>163</v>
       </c>
@@ -9877,7 +9878,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>167</v>
       </c>
@@ -9909,7 +9910,7 @@
         <v>44291</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>172</v>
       </c>
@@ -9941,7 +9942,7 @@
         <v>44317</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>177</v>
       </c>
@@ -9973,7 +9974,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>182</v>
       </c>
@@ -10005,7 +10006,7 @@
         <v>44391</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>187</v>
       </c>
@@ -10037,7 +10038,7 @@
         <v>44417</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>191</v>
       </c>
@@ -10069,7 +10070,7 @@
         <v>44443</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>197</v>
       </c>
@@ -10101,7 +10102,7 @@
         <v>44499</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>201</v>
       </c>
@@ -10133,7 +10134,7 @@
         <v>44525</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>207</v>
       </c>
@@ -10165,7 +10166,7 @@
         <v>44550</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>211</v>
       </c>
@@ -10197,7 +10198,7 @@
         <v>44249</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>217</v>
       </c>
@@ -10229,7 +10230,7 @@
         <v>44274</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>221</v>
       </c>
@@ -10261,7 +10262,7 @@
         <v>44300</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>226</v>
       </c>
@@ -10293,7 +10294,7 @@
         <v>44327</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>230</v>
       </c>
@@ -10325,7 +10326,7 @@
         <v>44353</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>157</v>
       </c>
@@ -10357,7 +10358,7 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>237</v>
       </c>
@@ -10389,7 +10390,7 @@
         <v>44435</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>243</v>
       </c>
@@ -10421,7 +10422,7 @@
         <v>44461</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>246</v>
       </c>
@@ -10453,7 +10454,7 @@
         <v>44487</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>250</v>
       </c>
@@ -10485,7 +10486,7 @@
         <v>44513</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>254</v>
       </c>
@@ -10517,7 +10518,7 @@
         <v>44539</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>243</v>
       </c>
@@ -10549,7 +10550,7 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>226</v>
       </c>
@@ -10581,7 +10582,7 @@
         <v>43881</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>19</v>
       </c>
@@ -10613,7 +10614,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>27</v>
       </c>
@@ -10645,7 +10646,7 @@
         <v>43933</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>35</v>
       </c>
@@ -10677,7 +10678,7 @@
         <v>43976</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>43</v>
       </c>
@@ -10709,7 +10710,7 @@
         <v>44000</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>50</v>
       </c>
@@ -10741,7 +10742,7 @@
         <v>44042</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>57</v>
       </c>
@@ -10773,7 +10774,7 @@
         <v>44057</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>254</v>
       </c>
@@ -10805,7 +10806,7 @@
         <v>44096</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>258</v>
       </c>
@@ -10837,7 +10838,7 @@
         <v>44113</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>364</v>
       </c>
@@ -10869,7 +10870,7 @@
         <v>44139</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>243</v>
       </c>
@@ -10901,7 +10902,7 @@
         <v>43858</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>64</v>
       </c>
@@ -10933,7 +10934,7 @@
         <v>43886</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>409</v>
       </c>
@@ -10965,7 +10966,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>271</v>
       </c>
@@ -10997,7 +10998,7 @@
         <v>43936</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>126</v>
       </c>
@@ -11029,7 +11030,7 @@
         <v>43981</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>115</v>
       </c>
@@ -11061,7 +11062,7 @@
         <v>44004</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>414</v>
       </c>
@@ -11093,7 +11094,7 @@
         <v>44029</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>151</v>
       </c>
@@ -11125,7 +11126,7 @@
         <v>44052</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>131</v>
       </c>
@@ -11157,7 +11158,7 @@
         <v>44076</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>100</v>
       </c>
@@ -11189,7 +11190,7 @@
         <v>44131</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>105</v>
       </c>
@@ -11221,7 +11222,7 @@
         <v>44157</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>157</v>
       </c>
@@ -11253,7 +11254,7 @@
         <v>44180</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>163</v>
       </c>
@@ -11285,7 +11286,7 @@
         <v>43842</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>167</v>
       </c>
@@ -11317,7 +11318,7 @@
         <v>43866</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>172</v>
       </c>
@@ -11349,7 +11350,7 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>177</v>
       </c>
@@ -11381,7 +11382,7 @@
         <v>43939</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>182</v>
       </c>
@@ -11413,7 +11414,7 @@
         <v>43965</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>187</v>
       </c>
@@ -11445,7 +11446,7 @@
         <v>43991</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>191</v>
       </c>
@@ -11477,7 +11478,7 @@
         <v>44016</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>197</v>
       </c>
@@ -11509,7 +11510,7 @@
         <v>44073</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>201</v>
       </c>
@@ -11541,7 +11542,7 @@
         <v>44099</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>207</v>
       </c>
@@ -11573,7 +11574,7 @@
         <v>44124</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>211</v>
       </c>
@@ -11605,7 +11606,7 @@
         <v>44157</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>217</v>
       </c>
@@ -11637,7 +11638,7 @@
         <v>44182</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>221</v>
       </c>
@@ -11669,7 +11670,7 @@
         <v>43841</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>226</v>
       </c>
@@ -11701,7 +11702,7 @@
         <v>43867</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>230</v>
       </c>
@@ -11733,7 +11734,7 @@
         <v>43893</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>157</v>
       </c>
@@ -11765,7 +11766,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>237</v>
       </c>
@@ -11797,7 +11798,7 @@
         <v>43977</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>243</v>
       </c>
@@ -11829,7 +11830,7 @@
         <v>44003</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>246</v>
       </c>
@@ -11861,7 +11862,7 @@
         <v>44028</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>250</v>
       </c>
@@ -11893,7 +11894,7 @@
         <v>44054</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>254</v>
       </c>
@@ -11925,7 +11926,7 @@
         <v>44080</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>243</v>
       </c>
@@ -11957,7 +11958,7 @@
         <v>43475</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>226</v>
       </c>
@@ -11989,7 +11990,7 @@
         <v>43516</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>19</v>
       </c>
@@ -12021,7 +12022,7 @@
         <v>43539</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>27</v>
       </c>
@@ -12053,7 +12054,7 @@
         <v>43567</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>35</v>
       </c>
@@ -12085,7 +12086,7 @@
         <v>43610</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>43</v>
       </c>
@@ -12117,7 +12118,7 @@
         <v>43634</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>50</v>
       </c>
@@ -12149,7 +12150,7 @@
         <v>43676</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>57</v>
       </c>
@@ -12181,7 +12182,7 @@
         <v>43691</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>254</v>
       </c>
@@ -12213,7 +12214,7 @@
         <v>43730</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>258</v>
       </c>
@@ -12245,7 +12246,7 @@
         <v>43747</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>364</v>
       </c>
@@ -12277,7 +12278,7 @@
         <v>43773</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>243</v>
       </c>
@@ -12309,7 +12310,7 @@
         <v>43493</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>64</v>
       </c>
@@ -12341,7 +12342,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>409</v>
       </c>
@@ -12373,7 +12374,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>271</v>
       </c>
@@ -12405,7 +12406,7 @@
         <v>43570</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>126</v>
       </c>
@@ -12437,7 +12438,7 @@
         <v>43615</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>115</v>
       </c>
@@ -12469,7 +12470,7 @@
         <v>43638</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>414</v>
       </c>
@@ -12501,7 +12502,7 @@
         <v>43663</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>151</v>
       </c>
@@ -12533,7 +12534,7 @@
         <v>43686</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>131</v>
       </c>
@@ -12565,7 +12566,7 @@
         <v>43710</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>100</v>
       </c>
@@ -12597,7 +12598,7 @@
         <v>43765</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>105</v>
       </c>
@@ -12629,7 +12630,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>157</v>
       </c>
@@ -12661,7 +12662,7 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>163</v>
       </c>
@@ -12693,7 +12694,7 @@
         <v>43477</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>167</v>
       </c>
@@ -12725,7 +12726,7 @@
         <v>43501</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>172</v>
       </c>
@@ -12757,7 +12758,7 @@
         <v>43525</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>177</v>
       </c>
@@ -12789,7 +12790,7 @@
         <v>43573</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>182</v>
       </c>
@@ -12821,7 +12822,7 @@
         <v>43599</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>187</v>
       </c>
@@ -12853,7 +12854,7 @@
         <v>43625</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>191</v>
       </c>
@@ -12885,7 +12886,7 @@
         <v>43650</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>197</v>
       </c>
@@ -12917,7 +12918,7 @@
         <v>43707</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>201</v>
       </c>
@@ -12949,7 +12950,7 @@
         <v>43733</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>207</v>
       </c>
@@ -12981,7 +12982,7 @@
         <v>43758</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>211</v>
       </c>
@@ -13013,7 +13014,7 @@
         <v>43791</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>217</v>
       </c>
@@ -13045,7 +13046,7 @@
         <v>43816</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>221</v>
       </c>
@@ -13077,7 +13078,7 @@
         <v>43476</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>226</v>
       </c>
@@ -13109,7 +13110,7 @@
         <v>43502</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>230</v>
       </c>
@@ -13141,7 +13142,7 @@
         <v>43527</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>157</v>
       </c>
@@ -13173,7 +13174,7 @@
         <v>43556</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>237</v>
       </c>
@@ -13205,7 +13206,7 @@
         <v>43611</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>243</v>
       </c>
@@ -13237,7 +13238,7 @@
         <v>43637</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>246</v>
       </c>
@@ -13269,7 +13270,7 @@
         <v>43662</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>250</v>
       </c>
@@ -13301,7 +13302,7 @@
         <v>43688</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>254</v>
       </c>

</xml_diff>